<commit_message>
End project with all results page working.
</commit_message>
<xml_diff>
--- a/data/DeftaultData.xlsx
+++ b/data/DeftaultData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabrielaServidone\Desktop\Gitlab\examples\application-examples\vessel-scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FF7E90-D375-425C-A23D-5EBE73AF552A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD06936-22A6-4A46-9E5C-9E957B00DF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" tabRatio="948" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16200" yWindow="2040" windowWidth="16410" windowHeight="15345" tabRatio="948" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Horizon" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,20 @@
     <sheet name="CargoData" sheetId="2" r:id="rId3"/>
     <sheet name="LocationData" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1209,7 +1222,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1269,7 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>16947</v>
+        <v>1694700</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -1279,7 +1292,7 @@
         <v>19</v>
       </c>
       <c r="D3">
-        <v>19181</v>
+        <v>1918100</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -1302,7 +1315,7 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>18465</v>
+        <v>1846500</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -1325,7 +1338,7 @@
         <v>28</v>
       </c>
       <c r="D5">
-        <v>12215</v>
+        <v>1221500</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
@@ -1348,7 +1361,7 @@
         <v>33</v>
       </c>
       <c r="D6">
-        <v>11210</v>
+        <v>1121000</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
@@ -1371,7 +1384,7 @@
         <v>38</v>
       </c>
       <c r="D7">
-        <v>13006</v>
+        <v>1300600</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -1394,7 +1407,7 @@
         <v>43</v>
       </c>
       <c r="D8">
-        <v>12757</v>
+        <v>1275700</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
@@ -1417,7 +1430,7 @@
         <v>47</v>
       </c>
       <c r="D9">
-        <v>10570</v>
+        <v>1057000</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -1440,7 +1453,7 @@
         <v>52</v>
       </c>
       <c r="D10">
-        <v>18900</v>
+        <v>1890000</v>
       </c>
       <c r="E10" t="s">
         <v>53</v>
@@ -1463,7 +1476,7 @@
         <v>37</v>
       </c>
       <c r="D11">
-        <v>16309</v>
+        <v>1630900</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -1486,7 +1499,7 @@
         <v>61</v>
       </c>
       <c r="D12">
-        <v>11811</v>
+        <v>1181100</v>
       </c>
       <c r="E12" t="s">
         <v>62</v>
@@ -1509,7 +1522,7 @@
         <v>65</v>
       </c>
       <c r="D13">
-        <v>14651</v>
+        <v>1465100</v>
       </c>
       <c r="E13" t="s">
         <v>66</v>
@@ -1532,7 +1545,7 @@
         <v>70</v>
       </c>
       <c r="D14">
-        <v>12041</v>
+        <v>1204100</v>
       </c>
       <c r="E14" t="s">
         <v>71</v>
@@ -1555,7 +1568,7 @@
         <v>75</v>
       </c>
       <c r="D15">
-        <v>11906</v>
+        <v>1190600</v>
       </c>
       <c r="E15" t="s">
         <v>58</v>
@@ -1578,7 +1591,7 @@
         <v>79</v>
       </c>
       <c r="D16">
-        <v>13943</v>
+        <v>1394300</v>
       </c>
       <c r="E16" t="s">
         <v>80</v>

</xml_diff>